<commit_message>
conduct 2d sinusoid PE experiments
</commit_message>
<xml_diff>
--- a/position_embedding_exp.xlsx
+++ b/position_embedding_exp.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csm81\Desktop\mnist_vit_1\vit_cifar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BE499E-0166-4B5E-A0CA-5C4A288018AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17CD67-CE27-491E-B522-5A3E51D75B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCF1F64B-F64B-4398-A119-8C30A5CF8D7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BCF1F64B-F64B-4398-A119-8C30A5CF8D7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>epoch</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sinusoid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>overfit -&gt;</t>
   </si>
   <si>
@@ -77,6 +74,42 @@
   </si>
   <si>
     <t>Loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length 65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Length 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no cls token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sinusoid 1d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sinusoid 2d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes cls token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -101,7 +134,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +153,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -135,7 +174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -143,6 +182,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -459,13 +501,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34AF7AD4-B89D-4DAF-A93C-826CEB0EE7D9}">
-  <dimension ref="A2:N16"/>
+  <dimension ref="A2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -613,228 +658,757 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>25</v>
-      </c>
-      <c r="H8">
-        <v>30</v>
-      </c>
-      <c r="I8">
-        <v>35</v>
-      </c>
-      <c r="J8">
-        <v>40</v>
-      </c>
-      <c r="K8">
-        <v>45</v>
-      </c>
-      <c r="L8">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>0.3468</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0.58169999999999999</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>0.64290000000000003</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>0.68810000000000004</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>0.71970000000000001</v>
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>0.74419999999999997</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>0.7601</v>
+        <v>30</v>
       </c>
       <c r="I9">
-        <v>0.76690000000000003</v>
+        <v>35</v>
       </c>
       <c r="J9">
-        <v>0.76990000000000003</v>
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.3468</v>
+      </c>
+      <c r="C10">
+        <v>0.58169999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.64290000000000003</v>
+      </c>
+      <c r="E10">
+        <v>0.68810000000000004</v>
+      </c>
+      <c r="F10">
+        <v>0.71970000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.74419999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.7601</v>
+      </c>
+      <c r="I10">
+        <v>0.76690000000000003</v>
+      </c>
+      <c r="J10">
+        <v>0.76990000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1.8162</v>
+      </c>
+      <c r="C11">
+        <v>1.1739999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.1023000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.87070000000000003</v>
+      </c>
+      <c r="F11">
+        <v>0.79069999999999996</v>
+      </c>
+      <c r="G11">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="H11">
+        <v>0.70779999999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="J11">
+        <v>0.87690000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
-      </c>
-      <c r="B10">
-        <v>1.8162</v>
-      </c>
-      <c r="C10">
-        <v>1.1739999999999999</v>
-      </c>
-      <c r="D10">
-        <v>1.1023000000000001</v>
-      </c>
-      <c r="E10">
-        <v>0.87070000000000003</v>
-      </c>
-      <c r="F10">
-        <v>0.79069999999999996</v>
-      </c>
-      <c r="G10">
-        <v>0.75929999999999997</v>
-      </c>
-      <c r="H10">
-        <v>0.70779999999999998</v>
-      </c>
-      <c r="I10">
-        <v>0.79200000000000004</v>
-      </c>
-      <c r="J10">
-        <v>0.87690000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <v>25</v>
-      </c>
-      <c r="H13">
-        <v>30</v>
-      </c>
-      <c r="I13">
-        <v>35</v>
-      </c>
-      <c r="J13">
-        <v>40</v>
-      </c>
-      <c r="K13">
-        <v>45</v>
-      </c>
-      <c r="L13">
-        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0.33350000000000002</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0.59140000000000004</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0.63819999999999999</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>0.67130000000000001</v>
+        <v>15</v>
       </c>
       <c r="F14">
-        <v>0.69679999999999997</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>0.72970000000000002</v>
+        <v>25</v>
       </c>
       <c r="H14">
-        <v>0.74339999999999995</v>
+        <v>30</v>
       </c>
       <c r="I14">
-        <v>0.75080000000000002</v>
+        <v>35</v>
       </c>
       <c r="J14">
-        <v>0.75260000000000005</v>
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <v>45</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0.33350000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.59140000000000004</v>
+      </c>
+      <c r="D15">
+        <v>0.63819999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.67130000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.69679999999999997</v>
+      </c>
+      <c r="G15">
+        <v>0.72970000000000002</v>
+      </c>
+      <c r="H15">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="I15">
+        <v>0.75080000000000002</v>
+      </c>
+      <c r="J15">
+        <v>0.75260000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1.9235</v>
+      </c>
+      <c r="C16">
+        <v>1.1513</v>
+      </c>
+      <c r="D16">
+        <v>1.0244</v>
+      </c>
+      <c r="E16">
+        <v>0.95369999999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.86219999999999997</v>
+      </c>
+      <c r="G16">
+        <v>0.77939999999999998</v>
+      </c>
+      <c r="H16">
+        <v>0.77949999999999997</v>
+      </c>
+      <c r="I16">
+        <v>0.79510000000000003</v>
+      </c>
+      <c r="J16">
+        <v>0.8377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
         <v>10</v>
       </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>35</v>
+      </c>
+      <c r="J19">
+        <v>40</v>
+      </c>
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.45129999999999998</v>
+      </c>
+      <c r="C20">
+        <v>0.60809999999999997</v>
+      </c>
+      <c r="D20">
+        <v>0.66490000000000005</v>
+      </c>
+      <c r="E20">
+        <v>0.6845</v>
+      </c>
+      <c r="F20">
+        <v>0.71289999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.73709999999999998</v>
+      </c>
+      <c r="H20">
+        <v>0.75</v>
+      </c>
+      <c r="I20">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="J20">
+        <v>0.76019999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1.5844</v>
+      </c>
+      <c r="C21">
+        <v>1.0851</v>
+      </c>
+      <c r="D21">
+        <v>0.94240000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.879</v>
+      </c>
+      <c r="F21">
+        <v>0.8196</v>
+      </c>
+      <c r="G21">
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="H21">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="I21">
+        <v>0.76149999999999995</v>
+      </c>
+      <c r="J21">
+        <v>0.80559999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650C016D-F916-429D-B57E-3E6633AE1E3D}">
+  <dimension ref="A6:R21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.41760000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="D10">
+        <v>0.64810000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.67130000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.69069999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.71809999999999996</v>
+      </c>
+      <c r="H10">
+        <v>0.73839999999999995</v>
+      </c>
+      <c r="I10">
+        <v>0.74639999999999995</v>
+      </c>
+      <c r="J10">
+        <v>0.76280000000000003</v>
+      </c>
+      <c r="K10">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L10">
+        <v>0.76519999999999999</v>
+      </c>
+      <c r="R10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1.6325000000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.1584000000000001</v>
+      </c>
+      <c r="D11">
+        <v>1.0012000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="F11">
+        <v>0.86460000000000004</v>
+      </c>
+      <c r="G11">
+        <v>0.79469999999999996</v>
+      </c>
+      <c r="H11">
+        <v>0.76349999999999996</v>
+      </c>
+      <c r="I11">
+        <v>0.7349</v>
+      </c>
+      <c r="J11">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="K11">
+        <v>0.70879999999999999</v>
+      </c>
+      <c r="L11">
+        <v>0.71009999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>35</v>
+      </c>
+      <c r="J14">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <v>45</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
       <c r="B15">
-        <v>1.9235</v>
+        <v>0.38729999999999998</v>
       </c>
       <c r="C15">
-        <v>1.1513</v>
+        <v>0.61990000000000001</v>
       </c>
       <c r="D15">
-        <v>1.0244</v>
+        <v>0.65749999999999997</v>
       </c>
       <c r="E15">
-        <v>0.95369999999999999</v>
+        <v>0.69179999999999997</v>
       </c>
       <c r="F15">
-        <v>0.86219999999999997</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="G15">
-        <v>0.77939999999999998</v>
+        <v>0.73380000000000001</v>
       </c>
       <c r="H15">
-        <v>0.77949999999999997</v>
+        <v>0.74860000000000004</v>
       </c>
       <c r="I15">
-        <v>0.79510000000000003</v>
+        <v>0.75790000000000002</v>
       </c>
       <c r="J15">
-        <v>0.8377</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
-        <v>8</v>
+        <v>0.76739999999999997</v>
+      </c>
+      <c r="K15">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="L15">
+        <v>0.77380000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1.7565</v>
+      </c>
+      <c r="C16">
+        <v>1.0653999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.96940000000000004</v>
+      </c>
+      <c r="E16">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="F16">
+        <v>0.85150000000000003</v>
+      </c>
+      <c r="G16">
+        <v>0.76739999999999997</v>
+      </c>
+      <c r="H16">
+        <v>0.7208</v>
+      </c>
+      <c r="I16">
+        <v>0.70089999999999997</v>
+      </c>
+      <c r="J16">
+        <v>0.68710000000000004</v>
+      </c>
+      <c r="K16">
+        <v>0.67989999999999995</v>
+      </c>
+      <c r="L16">
+        <v>0.68100000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>35</v>
+      </c>
+      <c r="J19">
+        <v>40</v>
+      </c>
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.39419999999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="D20">
+        <v>0.65390000000000004</v>
+      </c>
+      <c r="E20">
+        <v>0.68110000000000004</v>
+      </c>
+      <c r="F20">
+        <v>0.70040000000000002</v>
+      </c>
+      <c r="G20">
+        <v>0.72140000000000004</v>
+      </c>
+      <c r="H20">
+        <v>0.74050000000000005</v>
+      </c>
+      <c r="I20">
+        <v>0.75960000000000005</v>
+      </c>
+      <c r="J20">
+        <v>0.76839999999999997</v>
+      </c>
+      <c r="K20">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="L20">
+        <v>0.77429999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1.7155</v>
+      </c>
+      <c r="C21">
+        <v>1.1836</v>
+      </c>
+      <c r="D21">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="E21">
+        <v>0.9052</v>
+      </c>
+      <c r="F21">
+        <v>0.83660000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.78810000000000002</v>
+      </c>
+      <c r="H21">
+        <v>0.73819999999999997</v>
+      </c>
+      <c r="I21">
+        <v>0.71240000000000003</v>
+      </c>
+      <c r="J21">
+        <v>0.67349999999999999</v>
+      </c>
+      <c r="K21">
+        <v>0.67589999999999995</v>
+      </c>
+      <c r="L21">
+        <v>0.67530000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel for exp
</commit_message>
<xml_diff>
--- a/position_embedding_exp.xlsx
+++ b/position_embedding_exp.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csm81\Desktop\mnist_vit_1\vit_cifar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17CD67-CE27-491E-B522-5A3E51D75B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FABE23-DEE6-4C6C-932F-8CD7C1E347BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BCF1F64B-F64B-4398-A119-8C30A5CF8D7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BCF1F64B-F64B-4398-A119-8C30A5CF8D7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>epoch</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +113,49 @@
     <t>ss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>prod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overfitt-&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.8040(36) / 0.6297</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relative PE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Convit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overfitt-&gt;</t>
+  </si>
+  <si>
+    <t>Convit not init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no overfitting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +203,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -174,7 +224,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -185,6 +235,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -202,6 +255,2343 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>sinusoid 1d</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.3468</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64290000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68810000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.71970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74419999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.76690000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76990000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8CD-4734-A672-9032A6753C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.8162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1739999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1023000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87070000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79069999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75929999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.79200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.87690000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8CD-4734-A672-9032A6753C7F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1520241664"/>
+        <c:axId val="1520245824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1520241664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520245824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1520245824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520241664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>learnable</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.33350000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59140000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69679999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72970000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74339999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75080000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75260000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9419-4729-8353-0286357FEBD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.9235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0244</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77939999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77949999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.79510000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8377</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9419-4729-8353-0286357FEBD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1520937968"/>
+        <c:axId val="1520938800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1520937968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520938800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1520938800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520937968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E88C3AF-9B8E-2877-F608-D7AE0DACBEF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="차트 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A585A2A-CCF9-9782-6E68-7B2CFC4393E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>94780</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>199579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C82F473-9D98-EB1F-9482-A06739DE3AFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9363075" y="1028700"/>
+          <a:ext cx="3761905" cy="3571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>371019</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>37648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8B09EBC-7C38-8807-012B-FB6B35B786B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13182600" y="1028700"/>
+          <a:ext cx="3647619" cy="3619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,7 +2894,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1016,6 +3406,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1023,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650C016D-F916-429D-B57E-3E6633AE1E3D}">
   <dimension ref="A6:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1294,7 +3685,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1415,4 +3806,629 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF22ED2-575B-4887-AE5B-D0422E16BB48}">
+  <dimension ref="A6:M37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.30930000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.58020000000000005</v>
+      </c>
+      <c r="D10">
+        <v>0.64229999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.68159999999999998</v>
+      </c>
+      <c r="F10">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="G10">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="H10">
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.76259999999999994</v>
+      </c>
+      <c r="J10">
+        <v>0.78420000000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="L10">
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2.0863999999999998</v>
+      </c>
+      <c r="C11">
+        <v>1.177</v>
+      </c>
+      <c r="D11">
+        <v>1.0056</v>
+      </c>
+      <c r="E11">
+        <v>0.89419999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.84840000000000004</v>
+      </c>
+      <c r="G11">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="I11">
+        <v>0.68359999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.65780000000000005</v>
+      </c>
+      <c r="L11">
+        <v>0.65680000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>35</v>
+      </c>
+      <c r="J14">
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <v>45</v>
+      </c>
+      <c r="L14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>0.3952</v>
+      </c>
+      <c r="C15">
+        <v>0.58850000000000002</v>
+      </c>
+      <c r="D15">
+        <v>0.65810000000000002</v>
+      </c>
+      <c r="E15">
+        <v>0.7097</v>
+      </c>
+      <c r="F15">
+        <v>0.75170000000000003</v>
+      </c>
+      <c r="G15">
+        <v>0.77610000000000001</v>
+      </c>
+      <c r="H15">
+        <v>0.7923</v>
+      </c>
+      <c r="I15">
+        <v>0.79859999999999998</v>
+      </c>
+      <c r="J15">
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="K15">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="L15">
+        <v>0.81759999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1.8187</v>
+      </c>
+      <c r="C16">
+        <v>1.1438999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.82130000000000003</v>
+      </c>
+      <c r="F16">
+        <v>0.69389999999999996</v>
+      </c>
+      <c r="G16">
+        <v>0.65359999999999996</v>
+      </c>
+      <c r="H16">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.64329999999999998</v>
+      </c>
+      <c r="J16">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.70730000000000004</v>
+      </c>
+      <c r="L16">
+        <v>0.71150000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <v>35</v>
+      </c>
+      <c r="J19">
+        <v>40</v>
+      </c>
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.374</v>
+      </c>
+      <c r="C20">
+        <v>0.57789999999999997</v>
+      </c>
+      <c r="D20">
+        <v>0.65380000000000005</v>
+      </c>
+      <c r="E20">
+        <v>0.71009999999999995</v>
+      </c>
+      <c r="F20">
+        <v>0.75080000000000002</v>
+      </c>
+      <c r="G20">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="H20">
+        <v>0.7944</v>
+      </c>
+      <c r="I20">
+        <v>0.80310000000000004</v>
+      </c>
+      <c r="J20">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="K20">
+        <v>0.81810000000000005</v>
+      </c>
+      <c r="L20">
+        <v>0.81810000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1.8113999999999999</v>
+      </c>
+      <c r="C21">
+        <v>1.1942999999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.96689999999999998</v>
+      </c>
+      <c r="E21">
+        <v>0.82979999999999998</v>
+      </c>
+      <c r="F21">
+        <v>0.71640000000000004</v>
+      </c>
+      <c r="G21">
+        <v>0.67079999999999995</v>
+      </c>
+      <c r="H21">
+        <v>0.63029999999999997</v>
+      </c>
+      <c r="I21">
+        <v>0.61909999999999998</v>
+      </c>
+      <c r="J21">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="K21">
+        <v>0.68530000000000002</v>
+      </c>
+      <c r="L21">
+        <v>0.69140000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>30</v>
+      </c>
+      <c r="I26">
+        <v>35</v>
+      </c>
+      <c r="J26">
+        <v>40</v>
+      </c>
+      <c r="K26">
+        <v>45</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="M26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0.36070000000000002</v>
+      </c>
+      <c r="C27">
+        <v>0.52790000000000004</v>
+      </c>
+      <c r="D27">
+        <v>0.61209999999999998</v>
+      </c>
+      <c r="E27">
+        <v>0.71260000000000001</v>
+      </c>
+      <c r="F27">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0.80410000000000004</v>
+      </c>
+      <c r="H27">
+        <v>0.81979999999999997</v>
+      </c>
+      <c r="I27">
+        <v>0.83450000000000002</v>
+      </c>
+      <c r="J27">
+        <v>0.84870000000000001</v>
+      </c>
+      <c r="K27">
+        <v>0.84809999999999997</v>
+      </c>
+      <c r="L27">
+        <v>0.85209999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>1.7704</v>
+      </c>
+      <c r="C28">
+        <v>1.3063</v>
+      </c>
+      <c r="D28">
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0.81969999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="G28">
+        <v>0.55730000000000002</v>
+      </c>
+      <c r="H28">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="I28">
+        <v>0.48470000000000002</v>
+      </c>
+      <c r="J28">
+        <v>0.4546</v>
+      </c>
+      <c r="K28">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="L28">
+        <v>0.45810000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>0.5161</v>
+      </c>
+      <c r="D31">
+        <v>0.61260000000000003</v>
+      </c>
+      <c r="E31">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="F31">
+        <v>0.71630000000000005</v>
+      </c>
+      <c r="G31">
+        <v>0.74639999999999995</v>
+      </c>
+      <c r="H31">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="I31">
+        <v>0.8004</v>
+      </c>
+      <c r="J31">
+        <v>0.80840000000000001</v>
+      </c>
+      <c r="K31">
+        <v>0.81589999999999996</v>
+      </c>
+      <c r="L31">
+        <v>0.81859999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>0.54910000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>0.38019999999999998</v>
+      </c>
+      <c r="D37">
+        <v>0.57189999999999996</v>
+      </c>
+      <c r="E37">
+        <v>0.65229999999999999</v>
+      </c>
+      <c r="G37">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="H37">
+        <v>0.77529999999999999</v>
+      </c>
+      <c r="I37">
+        <v>0.7944</v>
+      </c>
+      <c r="J37">
+        <v>0.80810000000000004</v>
+      </c>
+      <c r="K37">
+        <v>0.81889999999999996</v>
+      </c>
+      <c r="L37">
+        <v>0.81540000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>